<commit_message>
add lab 1 video
</commit_message>
<xml_diff>
--- a/vignettes/course_docs/Schedule.xlsx
+++ b/vignettes/course_docs/Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattcrump/Github/psyc7709Lab/vignettes/course_docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF64B69-D3E8-7542-8481-186293B11E38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D2FDA05-DACE-C54D-A64A-0565DD491F0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17120" yWindow="460" windowWidth="16220" windowHeight="18940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -111,12 +111,6 @@
     <t>Semester Project IV</t>
   </si>
   <si>
-    <t>Lab 1 Descriptives</t>
-  </si>
-  <si>
-    <t>Lab 2 Variance and Transformed scores</t>
-  </si>
-  <si>
     <t>Lab 3 Distributions I</t>
   </si>
   <si>
@@ -151,6 +145,12 @@
   </si>
   <si>
     <t>TBD</t>
+  </si>
+  <si>
+    <t>Lab 1 Basics</t>
+  </si>
+  <si>
+    <t>Lab 2 Descriptives</t>
   </si>
 </sst>
 </file>
@@ -474,7 +474,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -511,10 +511,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -528,7 +528,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -542,7 +542,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
@@ -556,7 +556,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -581,7 +581,7 @@
         <v>10</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
         <v>3</v>
@@ -595,7 +595,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -609,7 +609,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D10" t="s">
         <v>5</v>
@@ -623,7 +623,7 @@
         <v>4</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
@@ -648,7 +648,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D13" t="s">
         <v>22</v>
@@ -662,7 +662,7 @@
         <v>22</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D14" t="s">
         <v>16</v>
@@ -695,7 +695,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D17" t="s">
         <v>17</v>
@@ -709,7 +709,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D18" t="s">
         <v>18</v>
@@ -726,7 +726,7 @@
         <v>26</v>
       </c>
       <c r="D19" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update syllabus and schedule
</commit_message>
<xml_diff>
--- a/vignettes/course_docs/Schedule.xlsx
+++ b/vignettes/course_docs/Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattcrump/Github/psyc7709Lab/vignettes/course_docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D2FDA05-DACE-C54D-A64A-0565DD491F0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{667AFD18-908D-C54B-AF9D-02C29F08254F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17120" yWindow="460" windowWidth="16220" windowHeight="18940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -147,10 +147,10 @@
     <t>TBD</t>
   </si>
   <si>
-    <t>Lab 1 Basics</t>
-  </si>
-  <si>
     <t>Lab 2 Descriptives</t>
+  </si>
+  <si>
+    <t>[Lab 1 Basics](https://crumplab.github.io/psyc7709Lab/articles/Lab1_Basics.html)</t>
   </si>
 </sst>
 </file>
@@ -474,7 +474,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -514,7 +514,7 @@
         <v>29</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -528,7 +528,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
update lab 4 on schedule
</commit_message>
<xml_diff>
--- a/vignettes/course_docs/Schedule.xlsx
+++ b/vignettes/course_docs/Schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattcrump/Github/psyc7709Lab/vignettes/course_docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0AFE37C-4E0C-D643-AD40-89C29FD76056}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8557DC00-FD0C-B343-AD0E-295C3417B354}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17120" yWindow="460" windowWidth="16220" windowHeight="18940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -111,9 +111,6 @@
     <t>Semester Project IV</t>
   </si>
   <si>
-    <t>Lab 4 Distributions II</t>
-  </si>
-  <si>
     <t>Th 27 Aug</t>
   </si>
   <si>
@@ -157,6 +154,9 @@
   </si>
   <si>
     <t>Th 3 Dec</t>
+  </si>
+  <si>
+    <t>[Lab 4 Distributions II](https://crumplab.github.io/psyc7709Lab/articles/Lab4_Distributions_II.html)</t>
   </si>
 </sst>
 </file>
@@ -480,7 +480,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -517,10 +517,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -534,7 +534,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -548,13 +548,13 @@
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -562,7 +562,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
@@ -587,7 +587,7 @@
         <v>10</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
         <v>3</v>
@@ -601,7 +601,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -615,10 +615,10 @@
         <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -629,7 +629,7 @@
         <v>4</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
@@ -654,7 +654,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13" t="s">
         <v>22</v>
@@ -668,10 +668,10 @@
         <v>22</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -701,7 +701,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D17" t="s">
         <v>17</v>
@@ -715,7 +715,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D18" t="s">
         <v>18</v>
@@ -732,7 +732,7 @@
         <v>26</v>
       </c>
       <c r="D19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add lab 5 youtubes
</commit_message>
<xml_diff>
--- a/vignettes/course_docs/Schedule.xlsx
+++ b/vignettes/course_docs/Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattcrump/Github/psyc7709Lab/vignettes/course_docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8CCA5D0-C77D-D64D-8FEE-F71078FA03C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBCF6CC6-80F9-4E44-8113-0DE50EC41E75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17120" yWindow="460" windowWidth="16220" windowHeight="18940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -114,9 +114,6 @@
     <t>Th 27 Aug</t>
   </si>
   <si>
-    <t>Lab 5 Distributions III</t>
-  </si>
-  <si>
     <t>Lab 6 Significance Testing</t>
   </si>
   <si>
@@ -157,13 +154,16 @@
   </si>
   <si>
     <t>[Lab 4 Distributions II](https://crumplab.github.io/psyc7709Lab/articles/Lab4_Distributions_II.html)</t>
+  </si>
+  <si>
+    <t>[Lab 5 Sampling Distributions](https://crumplab.github.io/psyc7709Lab/articles/Lab5_Sampling_Distributions.html)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -480,17 +480,17 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="71.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -504,7 +504,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="34">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -512,7 +512,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="17">
       <c r="A3">
         <v>1</v>
       </c>
@@ -520,13 +520,13 @@
         <v>27</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="51">
       <c r="A4">
         <v>2</v>
       </c>
@@ -534,13 +534,13 @@
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="34">
       <c r="A5">
         <v>3</v>
       </c>
@@ -548,13 +548,13 @@
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="34">
       <c r="A6">
         <v>4</v>
       </c>
@@ -562,13 +562,13 @@
         <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="17">
       <c r="A7">
         <v>5</v>
       </c>
@@ -579,7 +579,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="51">
       <c r="A8">
         <v>6</v>
       </c>
@@ -587,13 +587,13 @@
         <v>10</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="D8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="17">
       <c r="A9">
         <v>7</v>
       </c>
@@ -601,13 +601,13 @@
         <v>3</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="17">
       <c r="A10">
         <v>8</v>
       </c>
@@ -615,13 +615,13 @@
         <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="17">
       <c r="A11">
         <v>9</v>
       </c>
@@ -629,13 +629,13 @@
         <v>4</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="17">
       <c r="A12">
         <v>10</v>
       </c>
@@ -646,7 +646,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="17">
       <c r="A13">
         <v>11</v>
       </c>
@@ -654,13 +654,13 @@
         <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="17">
       <c r="A14">
         <v>12</v>
       </c>
@@ -668,13 +668,13 @@
         <v>22</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="17">
       <c r="A15">
         <v>13</v>
       </c>
@@ -685,7 +685,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="17">
       <c r="B16" t="s">
         <v>14</v>
       </c>
@@ -693,7 +693,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="17">
       <c r="A17">
         <v>14</v>
       </c>
@@ -701,13 +701,13 @@
         <v>16</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="17">
       <c r="A18">
         <v>15</v>
       </c>
@@ -715,13 +715,13 @@
         <v>17</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="17">
       <c r="A19">
         <v>16</v>
       </c>
@@ -732,7 +732,7 @@
         <v>26</v>
       </c>
       <c r="D19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>